<commit_message>
Adaboost with feature importance
</commit_message>
<xml_diff>
--- a/Summary Table.xlsx
+++ b/Summary Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t_velpac/mission/WorkingCopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D76B81-3011-A64C-BF61-78D2F540EF73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E08F93-6327-344D-984F-7D9F138E46E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{5E8CF062-5AA8-4146-81DF-556FDC69C932}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="17540" xr2:uid="{5E8CF062-5AA8-4146-81DF-556FDC69C932}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="36">
   <si>
     <t>(BEST)Standardized ANN (With Z-Scores- Deep and Wide)</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>MAE: DATA WITH TITLES</t>
+  </si>
+  <si>
+    <t>MSE:  Latest Data</t>
+  </si>
+  <si>
+    <t>MAE:  Latest Data</t>
   </si>
 </sst>
 </file>
@@ -399,8 +405,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5F91E3-23EA-9840-89E8-6FB4B9C99E2A}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,1629 +838,1714 @@
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="4" width="35.6640625" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="17" style="28" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="28" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="14.5" style="41" customWidth="1"/>
-    <col min="15" max="17" width="14.83203125" style="41" customWidth="1"/>
-    <col min="18" max="18" width="18.33203125" style="35" customWidth="1"/>
-    <col min="19" max="19" width="15" style="35" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" style="35" customWidth="1"/>
-    <col min="21" max="21" width="14.83203125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="21" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17" style="29" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="29" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="29" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="42" customWidth="1"/>
+    <col min="15" max="17" width="14.83203125" style="42" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" style="36" customWidth="1"/>
+    <col min="19" max="19" width="15" style="36" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" style="36" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" style="36" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="23" width="18.5" customWidth="1"/>
+    <col min="25" max="25" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:25" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42" t="s">
+      <c r="M1" s="43"/>
+      <c r="N1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42" t="s">
+      <c r="O1" s="43"/>
+      <c r="P1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42" t="s">
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42" t="s">
+      <c r="S1" s="43"/>
+      <c r="T1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="42"/>
-    </row>
-    <row r="2" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="45" t="s">
+      <c r="U1" s="43"/>
+      <c r="V1" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="43"/>
+    </row>
+    <row r="2" spans="1:25" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="45" t="s">
+      <c r="S2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="45" t="s">
+      <c r="T2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="45" t="s">
+      <c r="U2" s="46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="V2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="48">
         <v>0</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="48">
+      <c r="E3" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="49">
         <v>9.3015E-2</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="49">
         <v>4.1742000000000001E-2</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49">
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50">
         <v>3.8925000000000001E-2</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="50">
         <v>2.8625000000000001E-2</v>
       </c>
-      <c r="L3" s="49">
+      <c r="L3" s="50">
         <v>6.7347000000000004E-2</v>
       </c>
-      <c r="M3" s="49">
+      <c r="M3" s="50">
         <v>6.3116000000000005E-2</v>
       </c>
-      <c r="N3" s="54">
+      <c r="N3" s="55">
         <v>4.0825E-2</v>
       </c>
-      <c r="O3" s="54">
+      <c r="O3" s="55">
         <v>1.9671999999999999E-2</v>
       </c>
-      <c r="P3" s="54">
+      <c r="P3" s="55">
         <v>6.6616999999999996E-2</v>
       </c>
-      <c r="Q3" s="54">
+      <c r="Q3" s="55">
         <v>6.4907999999999993E-2</v>
       </c>
-      <c r="R3" s="50">
+      <c r="R3" s="51">
         <v>1.039134</v>
       </c>
-      <c r="S3" s="50">
+      <c r="S3" s="51">
         <v>0.93813899999999995</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-    </row>
-    <row r="4" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="47"/>
-      <c r="C4" s="46" t="s">
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="1">
+        <v>1.375991</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.90086999999999995</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.13569100000000001</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0.11106100000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="48"/>
+      <c r="C4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="48">
+      <c r="E4" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="49">
         <v>3.5394000000000002E-2</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="49">
         <v>3.9294999999999997E-2</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="49">
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50">
         <v>5.9727000000000002E-2</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="50">
         <v>7.2227E-2</v>
       </c>
-      <c r="L4" s="49">
+      <c r="L4" s="50">
         <v>0.120571</v>
       </c>
-      <c r="M4" s="49">
+      <c r="M4" s="50">
         <v>0.11450399999999999</v>
       </c>
-      <c r="N4" s="54">
+      <c r="N4" s="55">
         <v>5.2116000000000003E-2</v>
       </c>
-      <c r="O4" s="54">
+      <c r="O4" s="55">
         <v>5.8036999999999998E-2</v>
       </c>
-      <c r="P4" s="54">
+      <c r="P4" s="55">
         <v>8.6050000000000001E-2</v>
       </c>
-      <c r="Q4" s="54">
+      <c r="Q4" s="55">
         <v>8.5888000000000006E-2</v>
       </c>
-      <c r="R4" s="50">
+      <c r="R4" s="51">
         <v>1.0393159999999999</v>
       </c>
-      <c r="S4" s="50">
+      <c r="S4" s="51">
         <v>0.94352800000000003</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-    </row>
-    <row r="5" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="47"/>
-      <c r="C5" s="46" t="s">
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="1">
+        <v>1.380263</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.89980099999999996</v>
+      </c>
+      <c r="X4" s="1">
+        <v>9.9080000000000001E-2</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>7.3782E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="48"/>
+      <c r="C5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="48">
+      <c r="E5" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="49">
         <v>4.3668999999999999E-2</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="49">
         <v>3.6747000000000002E-2</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49">
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50">
         <v>7.5289999999999996E-2</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="50">
         <v>6.8792000000000006E-2</v>
       </c>
-      <c r="L5" s="49">
+      <c r="L5" s="50">
         <v>0.105238</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="50">
         <v>9.4992999999999994E-2</v>
       </c>
-      <c r="N5" s="54">
+      <c r="N5" s="55">
         <v>5.2248000000000003E-2</v>
       </c>
-      <c r="O5" s="54">
+      <c r="O5" s="55">
         <v>4.8966999999999997E-2</v>
       </c>
-      <c r="P5" s="54">
+      <c r="P5" s="55">
         <v>8.9099999999999999E-2</v>
       </c>
-      <c r="Q5" s="54">
+      <c r="Q5" s="55">
         <v>9.1004000000000002E-2</v>
       </c>
-      <c r="R5" s="50">
+      <c r="R5" s="51">
         <v>1.0389459999999999</v>
       </c>
-      <c r="S5" s="50">
+      <c r="S5" s="51">
         <v>0.93496400000000002</v>
       </c>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-    </row>
-    <row r="6" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="47"/>
-      <c r="C6" s="46" t="s">
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="1">
+        <v>1.3992329999999999</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1.606884</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0.196746</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0.17668600000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="48"/>
+      <c r="C6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="48">
+      <c r="E6" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="49">
         <v>7.9813999999999996E-2</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="49">
         <v>4.0696999999999997E-2</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49">
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50">
         <v>2.7559E-2</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="50">
         <v>2.1839000000000001E-2</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="50">
         <v>6.3235E-2</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="50">
         <v>6.1670999999999997E-2</v>
       </c>
-      <c r="N6" s="54">
+      <c r="N6" s="55">
         <v>3.7108000000000002E-2</v>
       </c>
-      <c r="O6" s="54">
+      <c r="O6" s="55">
         <v>2.3143E-2</v>
       </c>
-      <c r="P6" s="54">
+      <c r="P6" s="55">
         <v>6.8963999999999998E-2</v>
       </c>
-      <c r="Q6" s="54">
+      <c r="Q6" s="55">
         <v>6.1293E-2</v>
       </c>
-      <c r="R6" s="50">
+      <c r="R6" s="51">
         <v>1.0393790000000001</v>
       </c>
-      <c r="S6" s="50">
+      <c r="S6" s="51">
         <v>0.93784999999999996</v>
       </c>
-      <c r="T6" s="50"/>
-      <c r="U6" s="50"/>
-    </row>
-    <row r="7" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="47"/>
-      <c r="C7" s="46" t="s">
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="1">
+        <v>1.3811709999999999</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.899752</v>
+      </c>
+      <c r="X6" s="1">
+        <v>9.6698000000000006E-2</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>7.1648000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="48"/>
+      <c r="C7" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="48">
+      <c r="E7" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="49">
         <v>5.4165999999999999E-2</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="49">
         <v>2.5125999999999999E-2</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49">
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50">
         <v>3.4937999999999997E-2</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="50">
         <v>2.6525E-2</v>
       </c>
-      <c r="L7" s="49">
+      <c r="L7" s="50">
         <v>7.0551000000000003E-2</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="50">
         <v>6.9634000000000001E-2</v>
       </c>
-      <c r="N7" s="54">
+      <c r="N7" s="55">
         <v>7.0960999999999996E-2</v>
       </c>
-      <c r="O7" s="54">
+      <c r="O7" s="55">
         <v>5.6190999999999998E-2</v>
       </c>
-      <c r="P7" s="54">
+      <c r="P7" s="55">
         <v>8.0008999999999997E-2</v>
       </c>
-      <c r="Q7" s="54">
+      <c r="Q7" s="55">
         <v>7.8195000000000001E-2</v>
       </c>
-      <c r="R7" s="50">
+      <c r="R7" s="51">
         <v>1.04294</v>
       </c>
-      <c r="S7" s="50">
+      <c r="S7" s="51">
         <v>0.94676099999999996</v>
       </c>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-    </row>
-    <row r="8" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="1">
+        <v>1.379329</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.90156099999999995</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0.150814</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0.12585299999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="48">
         <v>0</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="48">
+      <c r="E8" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="49">
         <v>255.33720199999999</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="49">
         <v>1952.5570729999999</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="49">
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50">
         <v>44043.795592000002</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="50">
         <v>25805.846776999999</v>
       </c>
-      <c r="L8" s="49">
+      <c r="L8" s="50">
         <v>10.230976</v>
       </c>
-      <c r="M8" s="49">
+      <c r="M8" s="50">
         <v>8.3106329999999993</v>
       </c>
-      <c r="N8" s="51">
+      <c r="N8" s="52">
         <v>43870.418574000003</v>
       </c>
-      <c r="O8" s="54">
+      <c r="O8" s="55">
         <v>25282.149815000001</v>
       </c>
-      <c r="P8" s="54">
+      <c r="P8" s="55">
         <v>11.303791</v>
       </c>
-      <c r="Q8" s="54">
+      <c r="Q8" s="55">
         <v>9.2906870000000001</v>
       </c>
-      <c r="R8" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="S8" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-    </row>
-    <row r="9" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="47"/>
-      <c r="C9" s="53" t="s">
+      <c r="R8" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="S8" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+    </row>
+    <row r="9" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="48"/>
+      <c r="C9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="48">
+      <c r="E9" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="49">
         <v>267.55959100000001</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="49">
         <v>1967.6171870000001</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="49">
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50">
         <v>43830.496469999998</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="50">
         <v>25802.291436</v>
       </c>
-      <c r="L9" s="49">
+      <c r="L9" s="50">
         <v>11.603427999999999</v>
       </c>
-      <c r="M9" s="49">
+      <c r="M9" s="50">
         <v>9.7201389999999996</v>
       </c>
-      <c r="N9" s="54">
+      <c r="N9" s="55">
         <v>43873.429676</v>
       </c>
-      <c r="O9" s="54">
+      <c r="O9" s="55">
         <v>25809.388121</v>
       </c>
-      <c r="P9" s="54">
+      <c r="P9" s="55">
         <v>10.532045999999999</v>
       </c>
-      <c r="Q9" s="54">
+      <c r="Q9" s="55">
         <v>8.6586409999999994</v>
       </c>
-      <c r="R9" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="S9" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-    </row>
-    <row r="10" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="47"/>
-      <c r="C10" s="46" t="s">
+      <c r="R9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="53"/>
+      <c r="U9" s="53"/>
+    </row>
+    <row r="10" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="48"/>
+      <c r="C10" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="48">
+      <c r="E10" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="49">
         <v>247.65230199999999</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="49">
         <v>2044.8003799999999</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="49">
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50">
         <v>25944.232495</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="50">
         <v>25944.232495</v>
       </c>
-      <c r="L10" s="49">
+      <c r="L10" s="50">
         <v>8.4120919999999995</v>
       </c>
-      <c r="M10" s="49">
+      <c r="M10" s="50">
         <v>6.5727989999999998</v>
       </c>
-      <c r="N10" s="54">
+      <c r="N10" s="55">
         <v>44009.048009999999</v>
       </c>
-      <c r="O10" s="54">
+      <c r="O10" s="55">
         <v>25884.773667000001</v>
       </c>
-      <c r="P10" s="54">
+      <c r="P10" s="55">
         <v>9.1634139999999995</v>
       </c>
-      <c r="Q10" s="54">
+      <c r="Q10" s="55">
         <v>7.2828600000000003</v>
       </c>
-      <c r="R10" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="S10" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-    </row>
-    <row r="11" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="47"/>
-      <c r="C11" s="46" t="s">
+      <c r="R10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53"/>
+    </row>
+    <row r="11" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="48"/>
+      <c r="C11" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="48">
+      <c r="E11" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="49">
         <v>272.53551900000002</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="49">
         <v>2003.3451769999999</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="49">
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50">
         <v>43937.891477999998</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="50">
         <v>25762.955909</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="50">
         <v>10.694577000000001</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="50">
         <v>8.7565670000000004</v>
       </c>
-      <c r="N11" s="54">
+      <c r="N11" s="55">
         <v>43843.785370999998</v>
       </c>
-      <c r="O11" s="54">
+      <c r="O11" s="55">
         <v>25692.537251000002</v>
       </c>
-      <c r="P11" s="54">
+      <c r="P11" s="55">
         <v>11.223292000000001</v>
       </c>
-      <c r="Q11" s="51">
+      <c r="Q11" s="52">
         <v>9.3308180000000007</v>
       </c>
-      <c r="R11" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="S11" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-    </row>
-    <row r="12" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
-      <c r="C12" s="46" t="s">
+      <c r="R11" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="S11" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="53"/>
+      <c r="U11" s="53"/>
+    </row>
+    <row r="12" spans="1:25" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="48"/>
+      <c r="C12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="48">
+      <c r="E12" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="49">
         <v>311.48278499999998</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="49">
         <v>1951.743995</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="49">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50">
         <v>43909.182803999996</v>
       </c>
-      <c r="K12" s="49">
+      <c r="K12" s="50">
         <v>25785.574128</v>
       </c>
-      <c r="L12" s="49">
+      <c r="L12" s="50">
         <v>11.189266</v>
       </c>
-      <c r="M12" s="49">
+      <c r="M12" s="50">
         <v>9.3621909999999993</v>
       </c>
-      <c r="N12" s="54">
+      <c r="N12" s="55">
         <v>43932.901101000003</v>
       </c>
-      <c r="O12" s="54">
+      <c r="O12" s="55">
         <v>25655.804431</v>
       </c>
-      <c r="P12" s="54">
+      <c r="P12" s="55">
         <v>11.0253</v>
       </c>
-      <c r="Q12" s="54">
+      <c r="Q12" s="55">
         <v>9.0414720000000006</v>
       </c>
-      <c r="R12" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="S12" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="R12" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53"/>
+    </row>
+    <row r="13" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="21">
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="22">
         <v>0.16009599999999999</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="22">
         <v>0.113769</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="22">
         <v>0.116758</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="22">
         <v>0.108613</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="24">
         <v>0.13622999999999999</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="24">
         <v>0.12887100000000001</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="24">
         <v>0.132436</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="24">
         <v>0.130768</v>
       </c>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S13" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-    </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+    </row>
+    <row r="14" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="21">
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="22">
         <v>9.9926000000000001E-2</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="22">
         <v>3.9955999999999998E-2</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="22">
         <v>0.122431</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="22">
         <v>8.2822000000000007E-2</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="24">
         <v>7.8667000000000001E-2</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="24">
         <v>6.6739000000000007E-2</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="24">
         <v>0.10839699999999999</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="24">
         <v>0.107499</v>
       </c>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S14" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-    </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+    </row>
+    <row r="15" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>0</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="21">
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="22">
         <v>0.516235</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="22">
         <v>0.28916900000000001</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="22">
         <v>8.4683999999999995E-2</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="22">
         <v>6.2024000000000003E-2</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="24">
         <v>0.20447199999999999</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="24">
         <v>0.16217500000000001</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="5">
         <v>9.1213000000000002E-2</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="5">
         <v>7.7090000000000006E-2</v>
       </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S15" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-    </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+    </row>
+    <row r="16" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="21">
+      <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="22">
         <v>0.26746799999999998</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="23">
         <v>1.049408E-29</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="22">
         <v>5.7466999999999997E-2</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="23">
         <v>1.76922E-15</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="5">
         <v>9.7536999999999999E-2</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="6">
         <v>3.6998990000000001E-9</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="5">
         <v>6.9841E-2</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="5">
         <v>1.2E-5</v>
       </c>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
+      <c r="B17" s="2"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
+      <c r="B18" s="2"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-    </row>
-    <row r="20" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="B19" s="2"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+    </row>
+    <row r="20" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="12">
         <v>1</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="12">
+      <c r="E20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="13">
         <v>3.4921000000000001E-2</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="13">
         <v>2.1552000000000002E-2</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="13">
         <v>7.7289999999999998E-2</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="13">
         <v>5.9774000000000001E-2</v>
       </c>
-      <c r="N20" s="39">
+      <c r="N20" s="40">
         <v>4.8473000000000002E-2</v>
       </c>
-      <c r="O20" s="39">
+      <c r="O20" s="40">
         <v>2.3286000000000001E-2</v>
       </c>
-      <c r="P20" s="39">
+      <c r="P20" s="40">
         <v>8.4620000000000001E-2</v>
       </c>
-      <c r="Q20" s="39">
+      <c r="Q20" s="40">
         <v>6.3434000000000004E-2</v>
       </c>
-      <c r="R20" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-    </row>
-    <row r="21" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="10" t="s">
+      <c r="R20" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+    </row>
+    <row r="21" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="12">
+      <c r="E21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="13">
         <v>0.122485</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="13">
         <v>8.2110000000000002E-2</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="13">
         <v>0.11079600000000001</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="13">
         <v>9.0045E-2</v>
       </c>
-      <c r="N21" s="39">
+      <c r="N21" s="40">
         <v>4.4977999999999997E-2</v>
       </c>
-      <c r="O21" s="39">
+      <c r="O21" s="40">
         <v>3.7853999999999999E-2</v>
       </c>
-      <c r="P21" s="39">
+      <c r="P21" s="40">
         <v>9.1717000000000007E-2</v>
       </c>
-      <c r="Q21" s="39">
+      <c r="Q21" s="40">
         <v>7.8633999999999996E-2</v>
       </c>
-      <c r="R21" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S21" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-    </row>
-    <row r="22" spans="1:21" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="10" t="s">
+      <c r="R21" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" s="33"/>
+      <c r="U21" s="33"/>
+    </row>
+    <row r="22" spans="1:21" s="11" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="12">
+      <c r="E22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="13">
         <v>4.6018000000000003E-2</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="27">
         <v>83.476832000000002</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="13">
         <v>8.6349999999999996E-2</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="13">
         <v>0.112049</v>
       </c>
-      <c r="N22" s="39">
+      <c r="N22" s="40">
         <v>6.8200999999999998E-2</v>
       </c>
-      <c r="O22" s="39">
+      <c r="O22" s="40">
         <v>6.5124000000000001E-2</v>
       </c>
-      <c r="P22" s="39">
+      <c r="P22" s="40">
         <v>0.198158</v>
       </c>
-      <c r="Q22" s="39">
+      <c r="Q22" s="40">
         <v>0.19456100000000001</v>
       </c>
-      <c r="R22" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-    </row>
-    <row r="23" spans="1:21" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="10" t="s">
+      <c r="R22" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
+    </row>
+    <row r="23" spans="1:21" s="11" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="12">
+      <c r="E23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="13">
         <v>3.8894999999999999E-2</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="13">
         <v>2.5408E-2</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="13">
         <v>7.9208000000000001E-2</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="13">
         <v>6.157E-2</v>
       </c>
-      <c r="N23" s="39">
+      <c r="N23" s="40">
         <v>4.6578000000000001E-2</v>
       </c>
-      <c r="O23" s="39">
+      <c r="O23" s="40">
         <v>2.5071E-2</v>
       </c>
-      <c r="P23" s="39">
+      <c r="P23" s="40">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="Q23" s="39">
+      <c r="Q23" s="40">
         <v>6.4049999999999996E-2</v>
       </c>
-      <c r="R23" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S23" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-    </row>
-    <row r="24" spans="1:21" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="10" t="s">
+      <c r="R23" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+    </row>
+    <row r="24" spans="1:21" s="11" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="12">
+      <c r="E24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="13">
         <v>3.5393000000000001E-2</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="13">
         <v>2.6505000000000001E-2</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="13">
         <v>7.4115E-2</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M24" s="13">
         <v>6.7534999999999998E-2</v>
       </c>
-      <c r="N24" s="39">
+      <c r="N24" s="40">
         <v>3.1001000000000001E-2</v>
       </c>
-      <c r="O24" s="39">
+      <c r="O24" s="40">
         <v>2.6845000000000001E-2</v>
       </c>
-      <c r="P24" s="39">
+      <c r="P24" s="40">
         <v>7.2531999999999999E-2</v>
       </c>
-      <c r="Q24" s="39">
+      <c r="Q24" s="40">
         <v>6.8297999999999998E-2</v>
       </c>
-      <c r="R24" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S24" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-    </row>
-    <row r="25" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="R24" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+    </row>
+    <row r="25" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="12">
         <v>1</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="12">
+      <c r="E25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="13">
         <v>32933.049303</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="13">
         <v>28546.040433999999</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="13">
         <v>9.7802100000000003</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="13">
         <v>9.2720789999999997</v>
       </c>
-      <c r="N25" s="39">
+      <c r="N25" s="40">
         <v>32915.551848000003</v>
       </c>
-      <c r="O25" s="39">
+      <c r="O25" s="40">
         <v>28211.11334</v>
       </c>
-      <c r="P25" s="39">
+      <c r="P25" s="40">
         <v>11.162141</v>
       </c>
-      <c r="Q25" s="39">
+      <c r="Q25" s="40">
         <v>10.701815</v>
       </c>
-      <c r="R25" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S25" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-    </row>
-    <row r="26" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
-      <c r="C26" s="13" t="s">
+      <c r="R25" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S25" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+    </row>
+    <row r="26" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="12"/>
+      <c r="C26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="12">
+      <c r="E26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="13">
         <v>33037.701797000002</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="13">
         <v>28748.175735000001</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="13">
         <v>10.357562</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="13">
         <v>9.839988</v>
       </c>
-      <c r="N26" s="39">
+      <c r="N26" s="40">
         <v>32959.681398000001</v>
       </c>
-      <c r="O26" s="39">
+      <c r="O26" s="40">
         <v>28562.629271000002</v>
       </c>
-      <c r="P26" s="39">
+      <c r="P26" s="40">
         <v>11.41455</v>
       </c>
-      <c r="Q26" s="39">
+      <c r="Q26" s="40">
         <v>10.889141</v>
       </c>
-      <c r="R26" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T26" s="33"/>
-      <c r="U26" s="33"/>
-    </row>
-    <row r="27" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="11"/>
-      <c r="C27" s="10" t="s">
+      <c r="R26" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+    </row>
+    <row r="27" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="12"/>
+      <c r="C27" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="12">
+      <c r="E27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="13">
         <v>32979.752818000001</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="13">
         <v>28683.096979999998</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="13">
         <v>13.545287999999999</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="13">
         <v>13.012729999999999</v>
       </c>
-      <c r="N27" s="39">
+      <c r="N27" s="40">
         <v>32831.126888999999</v>
       </c>
-      <c r="O27" s="39">
+      <c r="O27" s="40">
         <v>28438.173879999998</v>
       </c>
-      <c r="P27" s="39">
+      <c r="P27" s="40">
         <v>10.394818000000001</v>
       </c>
-      <c r="Q27" s="39">
+      <c r="Q27" s="40">
         <v>9.8639030000000005</v>
       </c>
-      <c r="R27" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S27" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-    </row>
-    <row r="28" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="10" t="s">
+      <c r="R27" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+    </row>
+    <row r="28" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="12"/>
+      <c r="C28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="12">
+      <c r="E28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="13">
         <v>32895.983690000001</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="13">
         <v>28527.872543000001</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="13">
         <v>10.332288</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="13">
         <v>9.8276120000000002</v>
       </c>
-      <c r="N28" s="39">
+      <c r="N28" s="40">
         <v>33021.144748999999</v>
       </c>
-      <c r="O28" s="39">
+      <c r="O28" s="40">
         <v>28265.765256999999</v>
       </c>
-      <c r="P28" s="39">
+      <c r="P28" s="40">
         <v>9.7612509999999997</v>
       </c>
-      <c r="Q28" s="39">
+      <c r="Q28" s="40">
         <v>9.1675950000000004</v>
       </c>
-      <c r="R28" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S28" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
-    </row>
-    <row r="29" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="11"/>
-      <c r="C29" s="10" t="s">
+      <c r="R28" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+    </row>
+    <row r="29" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="12"/>
+      <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="12">
+      <c r="E29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="13">
         <v>32931.925503999999</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="13">
         <v>28534.217410000001</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="13">
         <v>11.045275999999999</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="13">
         <v>10.485970999999999</v>
       </c>
-      <c r="N29" s="39">
+      <c r="N29" s="40">
         <v>32982.715386000003</v>
       </c>
-      <c r="O29" s="39">
+      <c r="O29" s="40">
         <v>28414.568586000001</v>
       </c>
-      <c r="P29" s="39">
+      <c r="P29" s="40">
         <v>11.152006</v>
       </c>
-      <c r="Q29" s="39">
+      <c r="Q29" s="40">
         <v>10.580873</v>
       </c>
-      <c r="R29" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S29" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="T29" s="33"/>
-      <c r="U29" s="33"/>
-    </row>
-    <row r="30" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="R29" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+    </row>
+    <row r="30" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>1</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="18">
+      <c r="E30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="19">
         <v>0.19017999999999999</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="19">
         <v>9.7748000000000002E-2</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="19">
         <v>0.121237</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="19">
         <v>0.111652</v>
       </c>
-      <c r="J30" s="27">
+      <c r="J30" s="28">
         <v>0.13592599999999999</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="28">
         <v>0.130192</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="28">
         <v>0.13425400000000001</v>
       </c>
-      <c r="M30" s="27">
+      <c r="M30" s="28">
         <v>0.13147600000000001</v>
       </c>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="S30" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
-    </row>
-    <row r="31" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="S30" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
+    </row>
+    <row r="31" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="8">
         <v>1</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="18">
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="19">
         <v>9.7631999999999997E-2</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="19">
         <v>3.8996999999999997E-2</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="19">
         <v>0.105138</v>
       </c>
-      <c r="I31" s="18">
+      <c r="I31" s="19">
         <v>8.3737000000000006E-2</v>
       </c>
-      <c r="J31" s="27">
+      <c r="J31" s="28">
         <v>9.2422000000000004E-2</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="28">
         <v>6.7143999999999995E-2</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="28">
         <v>0.12392</v>
       </c>
-      <c r="M31" s="27">
+      <c r="M31" s="28">
         <v>0.107654</v>
       </c>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="S31" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
-    </row>
-    <row r="32" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="S31" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
+    </row>
+    <row r="32" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="8">
         <v>1</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="18">
+      <c r="E32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="19">
         <v>0.49954399999999999</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="19">
         <v>0.29253499999999999</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="19">
         <v>8.1082000000000001E-2</v>
       </c>
-      <c r="I32" s="18">
+      <c r="I32" s="19">
         <v>6.3544000000000003E-2</v>
       </c>
-      <c r="J32" s="27">
+      <c r="J32" s="28">
         <v>0.12525</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K32" s="28">
         <v>0.172955</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L32" s="9">
         <v>8.8513999999999995E-2</v>
       </c>
-      <c r="M32" s="8">
+      <c r="M32" s="9">
         <v>7.8141000000000002E-2</v>
       </c>
-      <c r="N32" s="40"/>
-      <c r="O32" s="40"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="S32" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
-    </row>
-    <row r="33" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+    </row>
+    <row r="33" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="8">
         <v>1</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="18">
+      <c r="E33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="19">
         <v>0.24931900000000001</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="20">
         <v>1.018959E-29</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="19">
         <v>4.1610000000000001E-2</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="20">
         <v>1.708714E-15</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="9">
         <v>0.108908</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="10">
         <v>3.599777E-9</v>
       </c>
-      <c r="L33" s="8">
+      <c r="L33" s="9">
         <v>8.5000999999999993E-2</v>
       </c>
-      <c r="M33" s="8">
+      <c r="M33" s="9">
         <v>1.2E-5</v>
       </c>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="S33" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="S33" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:E2"/>

</xml_diff>